<commit_message>
Actualizacion de manual de operaciones
</commit_message>
<xml_diff>
--- a/Entregables/Atributos de calidad.xlsx
+++ b/Entregables/Atributos de calidad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhone\Desktop\Entregables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyecto_Py\Cetaf_Python_Uikit_V1\Entregables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7284D3-2090-420E-9758-2EF9191169D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAD63C2-1933-4829-89BE-61D0DC3528F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,175 +28,135 @@
     <t>Descripción en el sistema</t>
   </si>
   <si>
+    <t>2. Disponibilidad.</t>
+  </si>
+  <si>
+    <t>3. Escalabilidad.</t>
+  </si>
+  <si>
+    <t>4. Interoperabilidad.</t>
+  </si>
+  <si>
+    <t>5. Modificabilidad.</t>
+  </si>
+  <si>
+    <t>6. Rendimiento.</t>
+  </si>
+  <si>
+    <t>7. Seguridad.</t>
+  </si>
+  <si>
+    <t>9. Usabilidad.</t>
+  </si>
+  <si>
+    <t>Aunque nuestro sistema no es un sistema complejo, cuenta con un framework que contiene diversos sistemas independientes, pueden ser incluidos si este fuere requerido. En django cuenta con un "Settings.py" donde se pueden instalar diversas Apps "INSTALLED_APPS" las cuales pueden integrarse.</t>
+  </si>
+  <si>
+    <t>El cliente  debe cumplir con un mínimo de requerimientos de software y hardware, una de las ventajas del sistemas, son los tiempos de respuesta ya que se encuentra desarrollado en Django, el cual es una herramienta ligera para el usuario.</t>
+  </si>
+  <si>
+    <t>A raíz de la implementación del framework Django, este cuenta con un sistema llamado "Shell". Shell es el intérprete interactivo de Python, que nos permitirá probar los modelos, hacer consultas, analizar resultados, antes de elaborar las vistas. Es muy útil si queremos ahorrar tiempo al momento de responder a los requerimientos que los usuarios de la aplicación puedan necesitar.</t>
+  </si>
+  <si>
+    <t>El software alberga un conjunto de pautas o elementos consiguiendo que la aplicación se amigable con el usuario, su interfaz es intuitiva , que permite al usuario aprender con  facilidad su funcionamiento.</t>
+  </si>
+  <si>
+    <t>Nuestro sistema permite que se pueda realizar cambios de acuerdo a las necesidades del cliente, los cambios o modificaciones que se realicen en el sistema van acorde a un cronograma al cual depende de la complejidad de los solicitado. Nuestro sistema ha sido desarrollado de tal forma que permite integrar nuevas funciones, es decir, en cada vista [Según el diseño de Django MVT] se implementa una clase principal la cual en un futuro puede hacer uso de funciones adicionales.</t>
+  </si>
+  <si>
+    <t>Nuestro sistema contiene diversos niveles de acceso que brinda seguridad, evitando ataques SQL, inyección de código,  perdida de autenticación, modificación en la carpetas. Habilita los accesos sólo a personal calificado que entienden del sistema, este se encuentra configurado definido por grupos, roles para los usuarios, restringiendo el acceso a los recursos según los roles.</t>
+  </si>
+  <si>
+    <t>Nuestro sistema se encuentra en una  arquitectura monolítico, con balanceador de carga, no contiene APis, por esta razón el cliente podrá implementar un escalamiento vertical, si este lo considera necesario.</t>
+  </si>
+  <si>
+    <t>El Sistema tiene la capacidad de estar disponible, una vez se haya presentado una falla determinada, es un sistema confiable, preparado para la recuperación  de desastres y  puede soportar fallas importantes.  Nuestro sistema tiene la capacidad de reaccionar cuando es ingresada una URL externa y este no se encuentra en el sistema.</t>
+  </si>
+  <si>
+    <t>Nuestro sistema será implementará localmente el en servidor del cliente, comunicado con los de mas equipos (PCs) a través de la red LAN, el cliente contratará con la empresa prestadora del internet una IP fija, la cual tendrá un enrutamiento desde la IP publica asignada por el proveedor de internet al puerto (8080). El cliente  debe cumplir con un mínimo de requerimientos de software y hardware, el cliente podrá conectarse remotamente desde una terminal externa(Internet) hacia la  IP del servidor.</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF686868"/>
-        <rFont val="Quattrocento Sans"/>
-      </rPr>
       <t>1. Desplegabilidad (</t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF686868"/>
-        <rFont val="Arial"/>
+        <rFont val="Ubuntu Light"/>
         <family val="2"/>
       </rPr>
       <t>facilidad de despliegue</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF686868"/>
-        <rFont val="Arial"/>
+        <rFont val="Ubuntu Light"/>
         <family val="2"/>
       </rPr>
       <t>).</t>
     </r>
   </si>
   <si>
-    <t>2. Disponibilidad.</t>
-  </si>
-  <si>
-    <t>3. Escalabilidad.</t>
-  </si>
-  <si>
-    <t>4. Interoperabilidad.</t>
-  </si>
-  <si>
-    <t>5. Modificabilidad.</t>
-  </si>
-  <si>
-    <t>6. Rendimiento.</t>
-  </si>
-  <si>
-    <t>7. Seguridad.</t>
-  </si>
-  <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF686868"/>
-        <rFont val="Quattrocento Sans"/>
-      </rPr>
       <t>8. Testeabilidad (</t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF686868"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Ubuntu Light"/>
         <family val="2"/>
       </rPr>
       <t>facilidad de probar el sistema</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF686868"/>
-        <rFont val="Segoe UI"/>
+        <rFont val="Ubuntu Light"/>
         <family val="2"/>
       </rPr>
       <t>).</t>
     </r>
-  </si>
-  <si>
-    <t>9. Usabilidad.</t>
-  </si>
-  <si>
-    <t>Aunque nuestro sistema no es un sistema complejo, cuenta con un framework que contiene diversos sistemas independientes, pueden ser incluidos si este fuere requerido. En django cuenta con un "Settings.py" donde se pueden instalar diversas Apps "INSTALLED_APPS" las cuales pueden integrarse.</t>
-  </si>
-  <si>
-    <t>El cliente  debe cumplir con un mínimo de requerimientos de software y hardware, una de las ventajas del sistemas, son los tiempos de respuesta ya que se encuentra desarrollado en Django, el cual es una herramienta ligera para el usuario.</t>
-  </si>
-  <si>
-    <t>A raíz de la implementación del framework Django, este cuenta con un sistema llamado "Shell". Shell es el intérprete interactivo de Python, que nos permitirá probar los modelos, hacer consultas, analizar resultados, antes de elaborar las vistas. Es muy útil si queremos ahorrar tiempo al momento de responder a los requerimientos que los usuarios de la aplicación puedan necesitar.</t>
-  </si>
-  <si>
-    <t>El software alberga un conjunto de pautas o elementos consiguiendo que la aplicación se amigable con el usuario, su interfaz es intuitiva , que permite al usuario aprender con  facilidad su funcionamiento.</t>
-  </si>
-  <si>
-    <t>Nuestro sistema permite que se pueda realizar cambios de acuerdo a las necesidades del cliente, los cambios o modificaciones que se realicen en el sistema van acorde a un cronograma al cual depende de la complejidad de los solicitado. Nuestro sistema ha sido desarrollado de tal forma que permite integrar nuevas funciones, es decir, en cada vista [Según el diseño de Django MVT] se implementa una clase principal la cual en un futuro puede hacer uso de funciones adicionales.</t>
-  </si>
-  <si>
-    <t>Nuestro sistema contiene diversos niveles de acceso que brinda seguridad, evitando ataques SQL, inyección de código,  perdida de autenticación, modificación en la carpetas. Habilita los accesos sólo a personal calificado que entienden del sistema, este se encuentra configurado definido por grupos, roles para los usuarios, restringiendo el acceso a los recursos según los roles.</t>
-  </si>
-  <si>
-    <t>Nuestro sistema se encuentra en una  arquitectura monolítico, con balanceador de carga, no contiene APis, por esta razón el cliente podrá implementar un escalamiento vertical, si este lo considera necesario.</t>
-  </si>
-  <si>
-    <t>El Sistema tiene la capacidad de estar disponible, una vez se haya presentado una falla determinada, es un sistema confiable, preparado para la recuperación  de desastres y  puede soportar fallas importantes.  Nuestro sistema tiene la capacidad de reaccionar cuando es ingresada una URL externa y este no se encuentra en el sistema.</t>
-  </si>
-  <si>
-    <t>Nuestro sistema será implementará localmente el en servidor del cliente, comunicado con los de mas equipos (PCs) a través de la red LAN, el cliente contratará con la empresa prestadora del internet una IP fija, la cual tendrá un enrutamiento desde la IP publica asignada por el proveedor de internet al puerto (8080). El cliente  debe cumplir con un mínimo de requerimientos de software y hardware, el cliente podrá conectarse remotamente desde una terminal externa(Internet) hacia la  IP del servidor.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF686868"/>
-      <name val="Quattrocento Sans"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Ubuntu Light"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Ubuntu Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF686868"/>
+      <name val="Ubuntu Light"/>
       <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF686868"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF686868"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF686868"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF686868"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Ubuntu Light"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -214,12 +174,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -232,42 +207,37 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,102 +456,101 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="18.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.75" customWidth="1"/>
-    <col min="4" max="26" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="82.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.75" style="1" customWidth="1"/>
+    <col min="4" max="26" width="9.375" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="87.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="123" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="66.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="41.25" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="68.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="81.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="75.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="72.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="84" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="71.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>